<commit_message>
REEMPLAZAR POR LA FECHA
</commit_message>
<xml_diff>
--- a/V SEMESTRE - CONTADURÍA PÚBLICA/PROCESOS CONTABLES III/1.EEFF COMPARATIVOS.xlsx
+++ b/V SEMESTRE - CONTADURÍA PÚBLICA/PROCESOS CONTABLES III/1.EEFF COMPARATIVOS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\V SEMESTRE - CONTADURÍA PÚBLICA\PROCESOS CONTABLES III\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86ECADF-E2BA-48F1-B073-B13306542278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ESF" sheetId="17" r:id="rId1"/>
@@ -21,24 +22,13 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">E.R.I.!$A$1:$H$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ESF!$A$1:$J$43</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="128">
   <si>
     <t>REPRESENTANTE LEGAL</t>
   </si>
@@ -379,12 +369,6 @@
     <t>COSTO DE VENTAS</t>
   </si>
   <si>
-    <t>Materiales construcción</t>
-  </si>
-  <si>
-    <t>MATERIALES DE CONSTRUCCIÓN</t>
-  </si>
-  <si>
     <t>Gastos administrativos</t>
   </si>
   <si>
@@ -392,24 +376,60 @@
   </si>
   <si>
     <t>Gastos financieros</t>
+  </si>
+  <si>
+    <t>GASTOS FINANCIEROS</t>
+  </si>
+  <si>
+    <t>Inventario</t>
+  </si>
+  <si>
+    <t>Recaudo cartera clientes</t>
+  </si>
+  <si>
+    <t>CLIENTES</t>
+  </si>
+  <si>
+    <t>INVENTARIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresos por ventas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gastos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margen Bruto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilidad del periodo </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="[$$-240A]\ #,##0"/>
+    <numFmt numFmtId="170" formatCode="[$$-240A]\ #,##0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,8 +524,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -518,8 +547,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -589,21 +624,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -637,61 +657,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -704,35 +827,35 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="9" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -746,22 +869,22 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -775,6 +898,59 @@
     <xf numFmtId="41" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="13" fillId="3" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="13" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -787,36 +963,22 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -838,10 +1000,74 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>996802</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>115397</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>443023</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>143982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect b="13104"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13279622" y="4490252"/>
+          <a:ext cx="5604244" cy="1158294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -879,9 +1105,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -916,7 +1142,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,7 +1177,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1124,11 +1350,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="P37" sqref="P37"/>
+    <sheetView showGridLines="0" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="AC45" sqref="AC45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1150,74 +1376,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
     </row>
     <row r="2" spans="1:13" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
     </row>
     <row r="3" spans="1:13" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
     </row>
     <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="119" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
     </row>
     <row r="6" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
@@ -1765,11 +1991,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,80 +2012,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="str">
+      <c r="A1" s="118" t="str">
         <f>+ESF!A1</f>
         <v>CIUDADELA INMOBILIARIA</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="str">
+      <c r="A2" s="118" t="str">
         <f>+ESF!A2</f>
         <v>NIT 910.926.298-8</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
     </row>
     <row r="3" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="str">
+      <c r="A4" s="120" t="str">
         <f>ESF!A4</f>
         <v>INFORMACION EN PESOS COLOMBIANOS</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="72" t="str">
+      <c r="A6" s="121" t="str">
         <f>+ESF!A5</f>
         <v>A DICIEMBRE 2022</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
     </row>
     <row r="7" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
@@ -2387,11 +2613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:M24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2433,18 +2659,17 @@
       <c r="B10" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="67"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="M11" s="67"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="65" t="s">
         <v>94</v>
       </c>
+      <c r="M12" s="68"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="65" t="s">
@@ -2461,19 +2686,25 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M18" s="68"/>
-    </row>
-    <row r="21" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:13" x14ac:dyDescent="0.3">
+      <c r="H19" s="67"/>
+    </row>
+    <row r="20" spans="8:13" x14ac:dyDescent="0.3">
+      <c r="H20" s="67"/>
+    </row>
+    <row r="21" spans="8:13" x14ac:dyDescent="0.3">
+      <c r="H21" s="67"/>
       <c r="M21" s="67"/>
     </row>
-    <row r="22" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:13" x14ac:dyDescent="0.3">
+      <c r="H22" s="67"/>
       <c r="M22" s="67"/>
     </row>
-    <row r="23" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:13" x14ac:dyDescent="0.3">
+      <c r="H23" s="67"/>
       <c r="M23" s="67"/>
     </row>
-    <row r="24" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:13" x14ac:dyDescent="0.3">
       <c r="M24" s="68"/>
     </row>
   </sheetData>
@@ -2482,97 +2713,102 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="P61" sqref="P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="1.28515625" customWidth="1"/>
+    <col min="16" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:22" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-    </row>
-    <row r="2" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+    </row>
+    <row r="2" spans="1:22" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="118" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-    </row>
-    <row r="3" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+    </row>
+    <row r="3" spans="1:22" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-    </row>
-    <row r="5" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+    </row>
+    <row r="5" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="119" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="119"/>
+      <c r="G5" s="119"/>
+      <c r="H5" s="119"/>
+      <c r="I5" s="119"/>
+      <c r="J5" s="119"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -2585,31 +2821,37 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="4"/>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="125" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="73"/>
-      <c r="J7" s="73" t="s">
+      <c r="H7" s="125"/>
+      <c r="J7" s="125" t="s">
         <v>101</v>
       </c>
-      <c r="K7" s="73"/>
-      <c r="M7" s="73" t="s">
+      <c r="K7" s="125"/>
+      <c r="M7" s="125" t="s">
         <v>111</v>
       </c>
-      <c r="N7" s="73"/>
-      <c r="P7" s="73" t="s">
+      <c r="N7" s="125"/>
+      <c r="P7" s="125" t="s">
         <v>112</v>
       </c>
-      <c r="Q7" s="73"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q7" s="125"/>
+      <c r="S7" s="122" t="s">
+        <v>102</v>
+      </c>
+      <c r="T7" s="123"/>
+      <c r="U7" s="123"/>
+      <c r="V7" s="124"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -2618,30 +2860,48 @@
       <c r="D8" s="4">
         <v>781827000</v>
       </c>
-      <c r="G8" s="74"/>
-      <c r="H8" s="75">
+      <c r="E8" s="77">
+        <f>J12</f>
+        <v>1727696000</v>
+      </c>
+      <c r="G8" s="69"/>
+      <c r="H8" s="70">
         <v>1850000000</v>
       </c>
       <c r="J8" s="78">
-        <f>I27</f>
-        <v>2201500000</v>
-      </c>
-      <c r="K8" s="90">
-        <f>J30</f>
+        <f>D8</f>
+        <v>781827000</v>
+      </c>
+      <c r="K8" s="76">
+        <f>V16</f>
         <v>1169770000</v>
       </c>
-      <c r="M8" s="78"/>
-      <c r="N8" s="86">
-        <f>J26</f>
-        <v>351500000</v>
-      </c>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="86">
-        <f>I28</f>
+      <c r="M8" s="83">
+        <f>U15</f>
+        <v>186770000</v>
+      </c>
+      <c r="N8" s="77">
+        <f>D36</f>
+        <v>25536000</v>
+      </c>
+      <c r="P8" s="102">
+        <f>U12</f>
         <v>1054499999.9999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S8" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T8" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="U8" s="79" t="s">
+        <v>105</v>
+      </c>
+      <c r="V8" s="79" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>86</v>
       </c>
@@ -2650,16 +2910,38 @@
       <c r="D9" s="4">
         <v>863500000</v>
       </c>
-      <c r="G9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="86">
-        <f>J32</f>
+      <c r="E9" s="70">
+        <f>P16</f>
+        <v>302225000</v>
+      </c>
+      <c r="G9" s="71"/>
+      <c r="J9" s="69">
+        <f>U11</f>
+        <v>2201500000</v>
+      </c>
+      <c r="K9" s="75">
+        <f>V18</f>
         <v>615856000</v>
       </c>
-      <c r="M9" s="76"/>
-      <c r="P9" s="76"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M9" s="71"/>
+      <c r="N9" s="75">
+        <f>V10</f>
+        <v>351500000</v>
+      </c>
+      <c r="P9" s="71"/>
+      <c r="S9" s="80">
+        <v>4135</v>
+      </c>
+      <c r="T9" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="U9" s="82"/>
+      <c r="V9" s="83">
+        <f>H8</f>
+        <v>1850000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -2668,12 +2950,41 @@
       <c r="D10" s="4">
         <v>22614000</v>
       </c>
-      <c r="G10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="M10" s="77"/>
-      <c r="P10" s="77"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E10" s="77">
+        <f>D10</f>
+        <v>22614000</v>
+      </c>
+      <c r="G10" s="72"/>
+      <c r="J10" s="71">
+        <f>U22</f>
+        <v>561275000</v>
+      </c>
+      <c r="K10" s="76">
+        <f>V20</f>
+        <v>31280000</v>
+      </c>
+      <c r="M10" s="129">
+        <f>SUM(M7:M9)</f>
+        <v>186770000</v>
+      </c>
+      <c r="N10" s="103">
+        <f>SUM(N7:N9)</f>
+        <v>377036000</v>
+      </c>
+      <c r="P10" s="72"/>
+      <c r="S10" s="84">
+        <v>2408</v>
+      </c>
+      <c r="T10" t="s">
+        <v>108</v>
+      </c>
+      <c r="U10" s="76"/>
+      <c r="V10" s="85">
+        <f>V9*19%</f>
+        <v>351500000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -2682,8 +2993,36 @@
       <c r="D11" s="4">
         <v>280774000</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E11" s="77">
+        <f>D11</f>
+        <v>280774000</v>
+      </c>
+      <c r="J11" s="103">
+        <f>SUM(J8:J10)</f>
+        <v>3544602000</v>
+      </c>
+      <c r="K11" s="106">
+        <f>SUM(K8:K10)</f>
+        <v>1816906000</v>
+      </c>
+      <c r="M11" s="72"/>
+      <c r="N11" s="128">
+        <f>N10-M10</f>
+        <v>190266000</v>
+      </c>
+      <c r="S11" s="84">
+        <v>1110</v>
+      </c>
+      <c r="T11" t="s">
+        <v>109</v>
+      </c>
+      <c r="U11" s="76">
+        <f>V9+V10</f>
+        <v>2201500000</v>
+      </c>
+      <c r="V11" s="85"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>89</v>
       </c>
@@ -2692,16 +3031,28 @@
       <c r="D12" s="11">
         <v>874507000</v>
       </c>
-      <c r="G12" s="73" t="s">
-        <v>114</v>
-      </c>
-      <c r="H12" s="73"/>
-      <c r="J12" s="73" t="s">
-        <v>116</v>
-      </c>
-      <c r="K12" s="73"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E12" s="77">
+        <f>G18</f>
+        <v>803007000.00000012</v>
+      </c>
+      <c r="J12" s="105">
+        <f>J11-K11</f>
+        <v>1727696000</v>
+      </c>
+      <c r="K12" s="84"/>
+      <c r="S12" s="86">
+        <v>6110</v>
+      </c>
+      <c r="T12" t="s">
+        <v>110</v>
+      </c>
+      <c r="U12" s="76">
+        <f>V9*57%</f>
+        <v>1054499999.9999999</v>
+      </c>
+      <c r="V12" s="85"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
@@ -2711,44 +3062,129 @@
         <f>SUM(D8:D12)</f>
         <v>2823222000</v>
       </c>
-      <c r="G13" s="74">
-        <f>I29</f>
-        <v>1169770000</v>
-      </c>
-      <c r="H13" s="75"/>
-      <c r="J13" s="78">
-        <f>I31</f>
-        <v>615856000</v>
-      </c>
-      <c r="K13" s="90"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E13" s="103">
+        <f>SUM(E8:E12)</f>
+        <v>3136316000</v>
+      </c>
+      <c r="S13" s="87">
+        <v>14</v>
+      </c>
+      <c r="T13" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="U13" s="88"/>
+      <c r="V13" s="89">
+        <f>U12</f>
+        <v>1054499999.9999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="58"/>
       <c r="C14" s="58"/>
       <c r="D14" s="4"/>
-      <c r="G14" s="76"/>
-      <c r="J14" s="76"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G14" s="125" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="125"/>
+      <c r="J14" s="125" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" s="125"/>
+      <c r="M14" s="125" t="s">
+        <v>116</v>
+      </c>
+      <c r="N14" s="125"/>
+      <c r="P14" s="125" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q14" s="125"/>
+      <c r="S14" s="90">
+        <v>14</v>
+      </c>
+      <c r="T14" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="U14" s="91">
+        <v>983000000</v>
+      </c>
+      <c r="V14" s="83"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="58"/>
       <c r="C15" s="58"/>
       <c r="D15" s="4"/>
-      <c r="G15" s="77"/>
-      <c r="J15" s="77"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G15" s="78">
+        <f>D12</f>
+        <v>874507000</v>
+      </c>
+      <c r="H15" s="70">
+        <f>V13</f>
+        <v>1054499999.9999999</v>
+      </c>
+      <c r="J15" s="73">
+        <f>U17</f>
+        <v>615856000</v>
+      </c>
+      <c r="K15" s="76"/>
+      <c r="M15" s="73">
+        <f>U19</f>
+        <v>31280000</v>
+      </c>
+      <c r="N15" s="76"/>
+      <c r="P15" s="108">
+        <f>D9</f>
+        <v>863500000</v>
+      </c>
+      <c r="Q15" s="109">
+        <f>V21</f>
+        <v>561275000</v>
+      </c>
+      <c r="S15" s="84">
+        <v>2408</v>
+      </c>
+      <c r="T15" t="s">
+        <v>108</v>
+      </c>
+      <c r="U15" s="100">
+        <f>U14*19%</f>
+        <v>186770000</v>
+      </c>
+      <c r="V15" s="101"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="58"/>
       <c r="C16" s="58"/>
       <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G16" s="69">
+        <f>U14</f>
+        <v>983000000</v>
+      </c>
+      <c r="J16" s="71"/>
+      <c r="M16" s="71"/>
+      <c r="P16" s="107">
+        <f>P15-Q15</f>
+        <v>302225000</v>
+      </c>
+      <c r="S16" s="92">
+        <v>1110</v>
+      </c>
+      <c r="T16" s="88" t="s">
+        <v>109</v>
+      </c>
+      <c r="U16" s="93"/>
+      <c r="V16" s="89">
+        <f>U14+U15</f>
+        <v>1169770000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>74</v>
       </c>
@@ -2757,8 +3193,33 @@
       <c r="D17" s="4">
         <v>462660000</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E17" s="77">
+        <f t="shared" ref="E17:E22" si="0">D17</f>
+        <v>462660000</v>
+      </c>
+      <c r="G17" s="127">
+        <f>SUM(G15:G16)</f>
+        <v>1857507000</v>
+      </c>
+      <c r="H17" s="126">
+        <f>SUM(H15)</f>
+        <v>1054499999.9999999</v>
+      </c>
+      <c r="J17" s="72"/>
+      <c r="M17" s="72"/>
+      <c r="P17" s="72"/>
+      <c r="S17" s="80">
+        <v>51</v>
+      </c>
+      <c r="T17" s="81" t="s">
+        <v>113</v>
+      </c>
+      <c r="U17" s="94">
+        <v>615856000</v>
+      </c>
+      <c r="V17" s="95"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -2767,8 +3228,27 @@
       <c r="D18" s="4">
         <v>366469000</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E18" s="77">
+        <f t="shared" si="0"/>
+        <v>366469000</v>
+      </c>
+      <c r="G18" s="105">
+        <f>G17-H17</f>
+        <v>803007000.00000012</v>
+      </c>
+      <c r="S18" s="92">
+        <v>1110</v>
+      </c>
+      <c r="T18" s="88" t="s">
+        <v>109</v>
+      </c>
+      <c r="U18" s="88"/>
+      <c r="V18" s="96">
+        <f>U17</f>
+        <v>615856000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -2777,8 +3257,22 @@
       <c r="D19" s="4">
         <v>16004000</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E19" s="77">
+        <f t="shared" si="0"/>
+        <v>16004000</v>
+      </c>
+      <c r="S19" s="80">
+        <v>5305</v>
+      </c>
+      <c r="T19" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="U19" s="97">
+        <v>31280000</v>
+      </c>
+      <c r="V19" s="83"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -2787,8 +3281,23 @@
       <c r="D20" s="4">
         <v>32608000</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E20" s="77">
+        <f t="shared" si="0"/>
+        <v>32608000</v>
+      </c>
+      <c r="S20" s="92">
+        <v>1110</v>
+      </c>
+      <c r="T20" s="88" t="s">
+        <v>109</v>
+      </c>
+      <c r="U20" s="88"/>
+      <c r="V20" s="89">
+        <f>U19</f>
+        <v>31280000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -2797,8 +3306,23 @@
       <c r="D21" s="4">
         <v>245190000</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="77">
+        <f t="shared" si="0"/>
+        <v>245190000</v>
+      </c>
+      <c r="S21" s="80">
+        <v>13</v>
+      </c>
+      <c r="T21" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="U21" s="81"/>
+      <c r="V21" s="78">
+        <f>D9*65%</f>
+        <v>561275000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -2807,8 +3331,23 @@
       <c r="D22" s="11">
         <v>-20057000</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E22" s="77">
+        <f t="shared" si="0"/>
+        <v>-20057000</v>
+      </c>
+      <c r="S22" s="92">
+        <v>1110</v>
+      </c>
+      <c r="T22" s="88" t="s">
+        <v>109</v>
+      </c>
+      <c r="U22" s="98">
+        <f>V21</f>
+        <v>561275000</v>
+      </c>
+      <c r="V22" s="99"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>30</v>
       </c>
@@ -2818,53 +3357,28 @@
         <f>SUM(D17:D22)</f>
         <v>1102874000</v>
       </c>
-      <c r="G23" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="H23" s="80"/>
-      <c r="I23" s="80"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E23" s="103">
+        <f>SUM(E17:E22)</f>
+        <v>1102874000</v>
+      </c>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="58"/>
       <c r="C24" s="58"/>
       <c r="D24" s="4"/>
-      <c r="G24" s="83" t="s">
-        <v>103</v>
-      </c>
-      <c r="H24" s="83" t="s">
-        <v>104</v>
-      </c>
-      <c r="I24" s="83" t="s">
-        <v>105</v>
-      </c>
-      <c r="J24" s="83" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B25" s="58"/>
       <c r="C25" s="58"/>
       <c r="D25" s="4"/>
-      <c r="G25">
-        <v>4135</v>
-      </c>
-      <c r="H25" t="s">
-        <v>107</v>
-      </c>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90">
-        <f>H8</f>
-        <v>1850000000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
@@ -2873,19 +3387,11 @@
       <c r="D26" s="4">
         <v>763000</v>
       </c>
-      <c r="G26">
-        <v>2408</v>
-      </c>
-      <c r="H26" s="84" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" s="90"/>
-      <c r="J26" s="91">
-        <f>J25*19%</f>
-        <v>351500000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E26" s="4">
+        <v>763000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
@@ -2894,19 +3400,11 @@
       <c r="D27" s="11">
         <v>-763000</v>
       </c>
-      <c r="G27">
-        <v>1110</v>
-      </c>
-      <c r="H27" s="84" t="s">
-        <v>109</v>
-      </c>
-      <c r="I27" s="90">
-        <f>J25+J26</f>
-        <v>2201500000</v>
-      </c>
-      <c r="J27" s="91"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E27" s="11">
+        <v>-763000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -2916,19 +3414,12 @@
         <f>SUM(D26:D27)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="87">
-        <v>6110</v>
-      </c>
-      <c r="H28" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="I28" s="90">
-        <f>J25*57%</f>
-        <v>1054499999.9999999</v>
-      </c>
-      <c r="J28" s="91"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="50">
+        <f>SUM(E26:E27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>4</v>
       </c>
@@ -2938,32 +3429,17 @@
         <f>+D13+D23+D28</f>
         <v>3926096000</v>
       </c>
-      <c r="G29" s="88">
-        <v>1405</v>
-      </c>
-      <c r="H29" s="84" t="s">
-        <v>113</v>
-      </c>
-      <c r="I29" s="89">
-        <f>(983000000*19%)+983000000</f>
-        <v>1169770000</v>
-      </c>
-      <c r="J29" s="90"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G30">
-        <v>1110</v>
-      </c>
-      <c r="H30" s="84" t="s">
-        <v>109</v>
-      </c>
-      <c r="I30" s="90"/>
-      <c r="J30" s="90">
-        <f>I29</f>
-        <v>1169770000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E29" s="20">
+        <f>+E13+E23+E28</f>
+        <v>4239190000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R30" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>6</v>
       </c>
@@ -2972,35 +3448,23 @@
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="54"/>
-      <c r="G31">
-        <v>51</v>
-      </c>
-      <c r="H31" s="84" t="s">
-        <v>115</v>
-      </c>
-      <c r="I31" s="85">
-        <v>615856000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="R31" t="s">
+        <v>122</v>
+      </c>
+      <c r="T31" s="76">
+        <f>V9</f>
+        <v>1850000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="1"/>
       <c r="D32" s="51"/>
-      <c r="G32">
-        <v>1110</v>
-      </c>
-      <c r="H32" s="84" t="s">
-        <v>109</v>
-      </c>
-      <c r="J32" s="86">
-        <f>I31</f>
-        <v>615856000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="43" t="s">
         <v>66</v>
       </c>
@@ -3009,18 +3473,15 @@
       <c r="D33" s="51">
         <v>287000</v>
       </c>
-      <c r="G33">
-        <v>5305</v>
-      </c>
-      <c r="H33" s="84" t="s">
-        <v>117</v>
-      </c>
-      <c r="I33" s="92">
-        <v>31280000</v>
-      </c>
-      <c r="J33" s="90"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E33" s="77">
+        <f>D33</f>
+        <v>287000</v>
+      </c>
+      <c r="R33" s="25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="43" t="s">
         <v>33</v>
       </c>
@@ -3029,20 +3490,38 @@
       <c r="D34" s="51">
         <v>178001000</v>
       </c>
-      <c r="I34" s="90"/>
-      <c r="J34" s="90"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="77">
+        <f>D34</f>
+        <v>178001000</v>
+      </c>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="R34" t="s">
+        <v>110</v>
+      </c>
+      <c r="T34" s="76">
+        <f>U12</f>
+        <v>1054499999.9999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="1"/>
       <c r="D35" s="51"/>
-      <c r="I35" s="90"/>
-      <c r="J35" s="90"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="76"/>
+      <c r="J35" s="76"/>
+      <c r="R35" s="112" t="s">
+        <v>125</v>
+      </c>
+      <c r="T35" s="113">
+        <f>T31-T34</f>
+        <v>795500000.00000012</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -3052,10 +3531,14 @@
         <f>9462000+1485000+14589000</f>
         <v>25536000</v>
       </c>
-      <c r="I36" s="90"/>
-      <c r="J36" s="90"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E36" s="77">
+        <f>N11</f>
+        <v>190266000</v>
+      </c>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -3065,10 +3548,17 @@
         <f>2039000+2925000+57000+24262000</f>
         <v>29283000</v>
       </c>
-      <c r="I37" s="90"/>
-      <c r="J37" s="90"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E37" s="77">
+        <f>D37</f>
+        <v>29283000</v>
+      </c>
+      <c r="I37" s="76"/>
+      <c r="J37" s="76"/>
+      <c r="R37" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
@@ -3077,8 +3567,18 @@
       <c r="D38" s="52">
         <v>18508000</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E38" s="77">
+        <f>D38</f>
+        <v>18508000</v>
+      </c>
+      <c r="R38" t="s">
+        <v>113</v>
+      </c>
+      <c r="T38" s="110">
+        <v>615856000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>12</v>
       </c>
@@ -3088,28 +3588,54 @@
         <f>SUM(D33:D38)</f>
         <v>251615000</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E39" s="103">
+        <f>SUM(E33:E38)</f>
+        <v>416345000</v>
+      </c>
+      <c r="R39" t="s">
+        <v>115</v>
+      </c>
+      <c r="T39" s="111">
+        <v>31280000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="9"/>
       <c r="C40" s="1"/>
       <c r="D40" s="51"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="R40" s="112" t="s">
+        <v>126</v>
+      </c>
+      <c r="S40" s="74"/>
+      <c r="T40" s="114">
+        <f>SUM(T38:T39)</f>
+        <v>647136000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="9"/>
       <c r="C41" s="1"/>
       <c r="D41" s="51"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="1"/>
       <c r="D42" s="51"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="R42" s="115" t="s">
+        <v>127</v>
+      </c>
+      <c r="S42" s="116"/>
+      <c r="T42" s="117">
+        <f>T35-T40</f>
+        <v>148364000.00000012</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="45" t="s">
         <v>66</v>
       </c>
@@ -3118,8 +3644,11 @@
       <c r="D43" s="51">
         <v>390643000</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E43" s="51">
+        <v>390643000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>75</v>
       </c>
@@ -3128,8 +3657,11 @@
       <c r="D44" s="52">
         <v>2158619000</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E44" s="52">
+        <v>2158619000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
@@ -3139,14 +3671,18 @@
         <f>SUM(D43:D44)</f>
         <v>2549262000</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E45" s="53">
+        <f>SUM(E43:E44)</f>
+        <v>2549262000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
       <c r="C46" s="1"/>
       <c r="D46" s="55"/>
     </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>8</v>
       </c>
@@ -3156,20 +3692,24 @@
         <f>+D39+D45</f>
         <v>2800877000</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="56">
+        <f>+E39+E45</f>
+        <v>2965607000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="9"/>
       <c r="C48" s="3"/>
       <c r="D48" s="62"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="14"/>
       <c r="C49" s="1"/>
       <c r="D49" s="51"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>1</v>
       </c>
@@ -3177,7 +3717,7 @@
       <c r="C50" s="1"/>
       <c r="D50" s="55"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
@@ -3186,8 +3726,11 @@
       <c r="D51" s="51">
         <v>843000000</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="51">
+        <v>843000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>48</v>
       </c>
@@ -3196,8 +3739,11 @@
       <c r="D52" s="51">
         <v>25309000</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="51">
+        <v>25309000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>73</v>
       </c>
@@ -3206,8 +3752,11 @@
       <c r="D53" s="51">
         <v>240171000</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="51">
+        <v>240171000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>13</v>
       </c>
@@ -3217,8 +3766,12 @@
         <f>E.R.I.!F48</f>
         <v>16739000</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="76">
+        <f>EJERCICIO!T42+D54</f>
+        <v>165103000.00000012</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="18"/>
       <c r="C55" s="1"/>
@@ -3226,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="44" t="s">
         <v>2</v>
       </c>
@@ -3236,20 +3789,24 @@
         <f>SUM(D51:D55)</f>
         <v>1125219000</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E56" s="104">
+        <f>SUM(E51:E54)</f>
+        <v>1273583000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="51"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="11"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>3</v>
       </c>
@@ -3259,24 +3816,31 @@
         <f>+D47+D56</f>
         <v>3926096000</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E59" s="15">
+        <f>+E47+E56</f>
+        <v>4239190000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="J12:K12"/>
+  <mergeCells count="14">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A5:J5"/>
+    <mergeCell ref="S7:V7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="J7:K7"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="P14:Q14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>